<commit_message>
varias coisa sei nem citar
</commit_message>
<xml_diff>
--- a/CheckList Projetos.xlsx
+++ b/CheckList Projetos.xlsx
@@ -493,7 +493,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -554,7 +554,7 @@
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C7" t="s">

</xml_diff>

<commit_message>
Chechlist atualizada e dificil de aturar checklist virou moda todo mundo quer usar
 :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100: :100:
</commit_message>
<xml_diff>
--- a/CheckList Projetos.xlsx
+++ b/CheckList Projetos.xlsx
@@ -179,11 +179,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -493,7 +492,7 @@
   <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -504,10 +503,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C1" t="s">
@@ -515,28 +514,28 @@
       </c>
     </row>
     <row r="2" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="5" t="s">
+      <c r="A2" s="5"/>
+      <c r="B2" s="4" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6"/>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="5"/>
+      <c r="B4" s="4" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C5" t="s">
@@ -544,8 +543,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="5"/>
+      <c r="B6" s="4" t="s">
         <v>4</v>
       </c>
       <c r="C6" t="s">
@@ -553,8 +552,8 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="5"/>
+      <c r="B7" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C7" t="s">
@@ -562,8 +561,8 @@
       </c>
     </row>
     <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="C8" t="s">
@@ -571,8 +570,8 @@
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="5"/>
+      <c r="B9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C9" t="s">
@@ -580,8 +579,8 @@
       </c>
     </row>
     <row r="10" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="5"/>
+      <c r="B10" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
@@ -589,8 +588,8 @@
       </c>
     </row>
     <row r="11" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="5" t="s">
+      <c r="A11" s="5"/>
+      <c r="B11" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C11" t="s">
@@ -598,8 +597,8 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
-      <c r="B12" s="5" t="s">
+      <c r="A12" s="5"/>
+      <c r="B12" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C12" t="s">
@@ -607,8 +606,8 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="3" t="s">
+      <c r="A13" s="5"/>
+      <c r="B13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C13" t="s">
@@ -616,40 +615,40 @@
       </c>
     </row>
     <row r="14" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6" t="s">
+      <c r="A14" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="4" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6"/>
-      <c r="B15" s="4" t="s">
+      <c r="A15" s="5"/>
+      <c r="B15" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="3" t="s">
+      <c r="A16" s="5"/>
+      <c r="B16" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="3" t="s">
+      <c r="A17" s="5"/>
+      <c r="B17" s="4" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="6"/>
-      <c r="B18" s="3" t="s">
+      <c r="A18" s="5"/>
+      <c r="B18" s="4" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="3" t="s">
+      <c r="A19" s="5"/>
+      <c r="B19" s="4" t="s">
         <v>23</v>
       </c>
     </row>

</xml_diff>